<commit_message>
updating affiliation and articles
</commit_message>
<xml_diff>
--- a/positions.xlsx
+++ b/positions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1da8a255b971a0b3/CV-gabrielnakamura/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{E8079C71-4F1B-4E04-972C-E6F1E6970344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{903A7C14-39E7-2643-BB12-5B65318C873D}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{E8079C71-4F1B-4E04-972C-E6F1E6970344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDD5AF95-BAFC-1843-8D1B-57FB521A6CCA}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19660" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="122">
   <si>
     <t>section</t>
   </si>
@@ -388,6 +388,15 @@
   </si>
   <si>
     <t>accepted in Neotropical Entomology</t>
+  </si>
+  <si>
+    <t>Herodotools: An R package to integrate macroevolution, biogeography, and community ecology</t>
+  </si>
+  <si>
+    <t>accepted for publication in Journal of Biogeography</t>
+  </si>
+  <si>
+    <t>**Nakamura G.** , Rodrigues AV., Luza ALL., Maestri R., Debastiani V. and Duarte L.</t>
   </si>
 </sst>
 </file>
@@ -929,6 +938,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1228,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1660,25 +1673,25 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D14" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
       </c>
       <c r="F14">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G14">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="H14" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="I14" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J14" t="s">
         <v>16</v>
@@ -1692,10 +1705,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="E15" t="s">
         <v>16</v>
@@ -1707,24 +1720,24 @@
         <v>2022</v>
       </c>
       <c r="H15" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="J15" t="s">
-        <v>114</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" t="s">
-        <v>11</v>
+      <c r="B16" t="b">
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="D16" t="s">
         <v>50</v>
@@ -1733,19 +1746,19 @@
         <v>16</v>
       </c>
       <c r="F16">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="G16">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="H16" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="I16" t="s">
         <v>16</v>
       </c>
       <c r="J16" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1756,13 +1769,13 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="F17">
         <v>2021</v>
@@ -1771,13 +1784,13 @@
         <v>2021</v>
       </c>
       <c r="H17" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I17" t="s">
         <v>16</v>
       </c>
       <c r="J17" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1785,13 +1798,13 @@
         <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
         <v>55</v>
@@ -1803,13 +1816,13 @@
         <v>2021</v>
       </c>
       <c r="H18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I18" t="s">
         <v>16</v>
       </c>
       <c r="J18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1820,10 +1833,10 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
         <v>55</v>
@@ -1835,13 +1848,13 @@
         <v>2021</v>
       </c>
       <c r="H19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I19" t="s">
         <v>16</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1852,10 +1865,10 @@
         <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
         <v>55</v>
@@ -1867,13 +1880,13 @@
         <v>2021</v>
       </c>
       <c r="H20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I20" t="s">
         <v>16</v>
       </c>
       <c r="J20" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1881,13 +1894,13 @@
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
         <v>55</v>
@@ -1899,7 +1912,7 @@
         <v>2021</v>
       </c>
       <c r="H21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I21" t="s">
         <v>16</v>
@@ -1913,25 +1926,25 @@
         <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E22" t="s">
         <v>55</v>
       </c>
       <c r="F22">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G22">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I22" t="s">
         <v>16</v>
@@ -1945,25 +1958,25 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
         <v>55</v>
       </c>
       <c r="F23">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="G23">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="H23" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I23" t="s">
         <v>16</v>
@@ -1977,25 +1990,25 @@
         <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
         <v>55</v>
       </c>
       <c r="F24">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="G24">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="H24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I24" t="s">
         <v>16</v>
@@ -2006,28 +2019,34 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="F25">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="G25">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="H25" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="I25" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -2038,10 +2057,10 @@
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
@@ -2053,13 +2072,7 @@
         <v>2021</v>
       </c>
       <c r="H26" t="s">
-        <v>86</v>
-      </c>
-      <c r="I26" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -2067,25 +2080,25 @@
         <v>81</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>
       </c>
       <c r="F27">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G27">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I27" t="s">
         <v>16</v>
@@ -2096,16 +2109,16 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E28" t="s">
         <v>16</v>
@@ -2117,10 +2130,10 @@
         <v>2020</v>
       </c>
       <c r="H28" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I28" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="J28" t="s">
         <v>16</v>
@@ -2134,7 +2147,7 @@
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
         <v>92</v>
@@ -2143,16 +2156,16 @@
         <v>16</v>
       </c>
       <c r="F29">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="G29">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="H29" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I29" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J29" t="s">
         <v>16</v>
@@ -2166,7 +2179,7 @@
         <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
         <v>92</v>
@@ -2175,16 +2188,16 @@
         <v>16</v>
       </c>
       <c r="F30">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="G30">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="H30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I30" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J30" t="s">
         <v>16</v>
@@ -2198,7 +2211,7 @@
         <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D31" t="s">
         <v>92</v>
@@ -2207,16 +2220,16 @@
         <v>16</v>
       </c>
       <c r="F31">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="G31">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="H31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J31" t="s">
         <v>16</v>
@@ -2224,31 +2237,31 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D32" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E32" t="s">
         <v>16</v>
       </c>
       <c r="F32">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="G32">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="H32" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="I32" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="J32" t="s">
         <v>16</v>
@@ -2262,7 +2275,7 @@
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="D33" t="s">
         <v>106</v>
@@ -2294,7 +2307,7 @@
         <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s">
         <v>106</v>
@@ -2302,11 +2315,11 @@
       <c r="E34" t="s">
         <v>16</v>
       </c>
-      <c r="F34" t="s">
-        <v>16</v>
+      <c r="F34">
+        <v>2021</v>
       </c>
       <c r="G34">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="H34" t="s">
         <v>16</v>
@@ -2326,7 +2339,7 @@
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D35" t="s">
         <v>106</v>
@@ -2358,7 +2371,7 @@
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D36" t="s">
         <v>106</v>
@@ -2390,7 +2403,7 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D37" t="s">
         <v>106</v>
@@ -2402,7 +2415,7 @@
         <v>16</v>
       </c>
       <c r="G37">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="H37" t="s">
         <v>16</v>
@@ -2422,7 +2435,7 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D38" t="s">
         <v>106</v>
@@ -2434,7 +2447,7 @@
         <v>16</v>
       </c>
       <c r="G38">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="H38" t="s">
         <v>16</v>
@@ -2454,7 +2467,7 @@
         <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="D39" t="s">
         <v>106</v>
@@ -2486,7 +2499,7 @@
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
         <v>106</v>
@@ -2498,7 +2511,7 @@
         <v>16</v>
       </c>
       <c r="G40">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="H40" t="s">
         <v>16</v>
@@ -2507,6 +2520,38 @@
         <v>16</v>
       </c>
       <c r="J40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" t="s">
+        <v>106</v>
+      </c>
+      <c r="E41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41">
+        <v>2021</v>
+      </c>
+      <c r="H41" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>